<commit_message>
login issue fixed, excel upload for marking text issue fixed in client module myorder
</commit_message>
<xml_diff>
--- a/src/assets/data/samplemarkingtext.xlsx
+++ b/src/assets/data/samplemarkingtext.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lapp project\lapp\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8037869D-7F8A-48FC-94DE-D0054A7249FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF1B74-D909-4344-A7A0-25A7A8CA01E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82E000C2-7093-487F-B01E-C704E9F98357}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{82E000C2-7093-487F-B01E-C704E9F98357}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,33 +30,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>L</t>
+    <t>Left Marking Text (L)</t>
   </si>
   <si>
-    <t>R</t>
+    <t>Others (O)</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>fvgbh</t>
-  </si>
-  <si>
-    <t>vb n</t>
-  </si>
-  <si>
-    <t>vgbhnjmk</t>
-  </si>
-  <si>
-    <t>fvgbhn</t>
-  </si>
-  <si>
-    <t>vfghn</t>
-  </si>
-  <si>
-    <t>fgbn</t>
+    <t>Right Marking Text  (R)</t>
   </si>
 </sst>
 </file>
@@ -417,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6B2080-5B5E-4DA4-86DA-10F95334E785}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,32 +418,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest API integrated and design changes for admin module for add, edit marking texts
</commit_message>
<xml_diff>
--- a/src/assets/data/samplemarkingtext.xlsx
+++ b/src/assets/data/samplemarkingtext.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lapp project\lapp\src\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lapp\Production\lapp\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF1B74-D909-4344-A7A0-25A7A8CA01E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A1CAB3-865A-4C2B-B2E4-59D54363EAE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{82E000C2-7093-487F-B01E-C704E9F98357}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82E000C2-7093-487F-B01E-C704E9F98357}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>Left Marking Text (L)</t>
   </si>
@@ -39,13 +39,22 @@
   </si>
   <si>
     <t>Right Marking Text  (R)</t>
+  </si>
+  <si>
+    <t>RM Part No L</t>
+  </si>
+  <si>
+    <t>RM Part No R</t>
+  </si>
+  <si>
+    <t>RM Part No O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +69,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,9 +98,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6B2080-5B5E-4DA4-86DA-10F95334E785}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,10 +432,12 @@
     <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="30.44140625" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,6 +446,15 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>